<commit_message>
updated use case estimation diagram
</commit_message>
<xml_diff>
--- a/Metadata/FPs_with_plot2.xlsx
+++ b/Metadata/FPs_with_plot2.xlsx
@@ -548,35 +548,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,6 +736,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>New Use Cases</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -790,11 +793,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="100741888"/>
-        <c:axId val="100743808"/>
+        <c:axId val="100789632"/>
+        <c:axId val="100877824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100741888"/>
+        <c:axId val="100789632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,12 +823,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100743808"/>
+        <c:crossAx val="100877824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100743808"/>
+        <c:axId val="100877824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +855,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100741888"/>
+        <c:crossAx val="100789632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -865,7 +868,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1193,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1208,32 +1211,32 @@
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28" t="s">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="26.25" thickBot="1">
-      <c r="A4" s="22"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1246,8 +1249,8 @@
       <c r="G4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9" ht="26.25" thickBot="1">
       <c r="A5" s="5">

</xml_diff>